<commit_message>
Update sample data generation with 5 projects and nested structure
</commit_message>
<xml_diff>
--- a/public/sample_data.xlsx
+++ b/public/sample_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="177">
   <si>
     <t>Name</t>
   </si>
@@ -58,52 +58,118 @@
     <t>Man Days Actual</t>
   </si>
   <si>
-    <t>Digital Transformation 2025</t>
-  </si>
-  <si>
-    <t>Overhaul of legacy systems and migration to cloud</t>
+    <t>Cloud Migration 2025</t>
+  </si>
+  <si>
+    <t>Strategic initiative for Infrastructure</t>
   </si>
   <si>
     <t>John Doe</t>
   </si>
   <si>
+    <t>PM John</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Infrastructure</t>
+  </si>
+  <si>
+    <t>Vendor A</t>
+  </si>
+  <si>
+    <t>contact@vendorA.com</t>
+  </si>
+  <si>
+    <t>AI Customer Support</t>
+  </si>
+  <si>
+    <t>Strategic initiative for Innovation</t>
+  </si>
+  <si>
     <t>Alice Smith</t>
   </si>
   <si>
+    <t>PM Alice</t>
+  </si>
+  <si>
     <t>In Progress</t>
   </si>
   <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>TechCorp</t>
-  </si>
-  <si>
-    <t>sales@techcorp.com</t>
-  </si>
-  <si>
-    <t>Mobile App Revamp</t>
-  </si>
-  <si>
-    <t>Redesign of customer facing mobile application</t>
+    <t>Innovation</t>
+  </si>
+  <si>
+    <t>Vendor B</t>
+  </si>
+  <si>
+    <t>contact@vendorB.com</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit</t>
+  </si>
+  <si>
+    <t>Strategic initiative for Security</t>
+  </si>
+  <si>
+    <t>Bob Jones</t>
+  </si>
+  <si>
+    <t>PM Bob</t>
+  </si>
+  <si>
+    <t>On Hold</t>
+  </si>
+  <si>
+    <t>Security</t>
+  </si>
+  <si>
+    <t>Vendor C</t>
+  </si>
+  <si>
+    <t>contact@vendorC.com</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign</t>
+  </si>
+  <si>
+    <t>Strategic initiative for Product</t>
   </si>
   <si>
     <t>Jane Roe</t>
   </si>
   <si>
-    <t>Bob Jones</t>
-  </si>
-  <si>
-    <t>Planning</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>AppStudio</t>
-  </si>
-  <si>
-    <t>contact@appstudio.com</t>
+    <t>PM Jane</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Vendor D</t>
+  </si>
+  <si>
+    <t>contact@vendorD.com</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp</t>
+  </si>
+  <si>
+    <t>Strategic initiative for Data</t>
+  </si>
+  <si>
+    <t>Mike Data</t>
+  </si>
+  <si>
+    <t>PM Mike</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Vendor E</t>
+  </si>
+  <si>
+    <t>contact@vendorE.com</t>
   </si>
   <si>
     <t>Project Name</t>
@@ -112,22 +178,40 @@
     <t>Budget</t>
   </si>
   <si>
-    <t>Migrate Core Database</t>
-  </si>
-  <si>
-    <t>Mike Database</t>
-  </si>
-  <si>
-    <t>Implement New CRM</t>
-  </si>
-  <si>
-    <t>Sarah Sales</t>
-  </si>
-  <si>
-    <t>UI/UX Redesign</t>
-  </si>
-  <si>
-    <t>Designer Dan</t>
+    <t>Cloud Migration 2025 - Goal 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2</t>
   </si>
   <si>
     <t>Goal Description</t>
@@ -136,22 +220,115 @@
     <t>Timeline</t>
   </si>
   <si>
-    <t>Schema Design</t>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 1</t>
+  </si>
+  <si>
+    <t>Lead 1</t>
   </si>
   <si>
     <t>Q1 2025</t>
   </si>
   <si>
-    <t>Data Migration Scripts</t>
-  </si>
-  <si>
-    <t>Dev Dave</t>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 2</t>
+  </si>
+  <si>
+    <t>Lead 2</t>
   </si>
   <si>
     <t>Q2 2025</t>
   </si>
   <si>
-    <t>Vendor Selection</t>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 3</t>
+  </si>
+  <si>
+    <t>Lead 3</t>
+  </si>
+  <si>
+    <t>Q3 2025</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 3</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 3</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 2</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 3</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 3</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 3</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 2</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 3</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 2</t>
   </si>
   <si>
     <t>Scope Description(s)</t>
@@ -160,19 +337,214 @@
     <t>Assignee</t>
   </si>
   <si>
-    <t>ERD Diagram</t>
-  </si>
-  <si>
-    <t>Architect Ann</t>
-  </si>
-  <si>
-    <t>Database Setup Scripts</t>
-  </si>
-  <si>
-    <t>ETL Pipeline</t>
-  </si>
-  <si>
-    <t>Data Don</t>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Dev 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Dev 2</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Dev 3</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 1 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Cloud Migration 2025 - Goal 2 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 1 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 2 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>AI Customer Support - Goal 3 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 1 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Enterprise Security Audit - Goal 2 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 1 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 2 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Mobile App Redesign - Goal 3 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 2 - Deliverable 3</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 1 - Scope 3 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 1 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 1 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 2 - Deliverable 1</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 2 - Deliverable 2</t>
+  </si>
+  <si>
+    <t>Data Warehouse Revamp - Goal 2 - Scope 2 - Deliverable 3</t>
   </si>
 </sst>
 </file>
@@ -559,7 +931,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N6"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -636,10 +1008,10 @@
         <v>19</v>
       </c>
       <c r="G2">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="H2">
-        <v>150000</v>
+        <v>20000</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -651,13 +1023,13 @@
         <v>21</v>
       </c>
       <c r="L2">
-        <v>200000</v>
+        <v>50000</v>
       </c>
       <c r="M2">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="N2">
-        <v>250</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -680,10 +1052,10 @@
         <v>27</v>
       </c>
       <c r="G3">
-        <v>150000</v>
+        <v>200000</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -698,10 +1070,142 @@
         <v>100000</v>
       </c>
       <c r="M3">
+        <v>200</v>
+      </c>
+      <c r="N3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4">
+        <v>300000</v>
+      </c>
+      <c r="H4">
+        <v>60000</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L4">
+        <v>150000</v>
+      </c>
+      <c r="M4">
         <v>300</v>
       </c>
-      <c r="N3">
+      <c r="N4">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5">
+        <v>400000</v>
+      </c>
+      <c r="H5">
+        <v>80000</v>
+      </c>
+      <c r="I5">
         <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5">
+        <v>200000</v>
+      </c>
+      <c r="M5">
+        <v>400</v>
+      </c>
+      <c r="N5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6">
+        <v>500000</v>
+      </c>
+      <c r="H6">
+        <v>100000</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" t="s">
+        <v>51</v>
+      </c>
+      <c r="L6">
+        <v>250000</v>
+      </c>
+      <c r="M6">
+        <v>500</v>
+      </c>
+      <c r="N6">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -712,7 +1216,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
@@ -723,7 +1227,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -732,7 +1236,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -740,13 +1244,13 @@
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="D2">
-        <v>100000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -754,13 +1258,13 @@
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>16</v>
       </c>
       <c r="D3">
-        <v>200000</v>
+        <v>30000</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -768,13 +1272,139 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>50000</v>
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>
@@ -785,7 +1415,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E32"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="50" customWidth="1"/>
@@ -796,7 +1426,7 @@
   <sheetData>
     <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -805,61 +1435,537 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="D2">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="D3">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="E3" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="D4">
         <v>10000</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5">
+        <v>10000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6">
+        <v>10000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7">
+        <v>10000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8">
+        <v>10000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10">
+        <v>10000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11">
+        <v>10000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13">
+        <v>10000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14">
+        <v>10000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>69</v>
+      </c>
+      <c r="D15">
+        <v>10000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16">
+        <v>10000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17">
+        <v>10000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18">
+        <v>10000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19">
+        <v>10000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20">
+        <v>10000</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21">
+        <v>10000</v>
+      </c>
+      <c r="E21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B22" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22">
+        <v>10000</v>
+      </c>
+      <c r="E22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23">
+        <v>10000</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>96</v>
+      </c>
+      <c r="C24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D24">
+        <v>10000</v>
+      </c>
+      <c r="E24" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25">
+        <v>10000</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C26" t="s">
+        <v>72</v>
+      </c>
+      <c r="D26">
+        <v>10000</v>
+      </c>
+      <c r="E26" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>63</v>
+      </c>
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="C27" t="s">
+        <v>75</v>
+      </c>
+      <c r="D27">
+        <v>10000</v>
+      </c>
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28">
+        <v>10000</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C29" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29">
+        <v>10000</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30">
+        <v>10000</v>
+      </c>
+      <c r="E30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31">
+        <v>10000</v>
+      </c>
+      <c r="E31" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>65</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32">
+        <v>10000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -870,7 +1976,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F68"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="50" customWidth="1"/>
@@ -881,19 +1987,19 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>47</v>
+        <v>106</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -901,62 +2007,1342 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>108</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
       <c r="E2">
         <v>5000</v>
       </c>
       <c r="F2">
-        <v>100</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3">
+        <v>5000</v>
+      </c>
+      <c r="F3">
         <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E3">
-        <v>15000</v>
-      </c>
-      <c r="F3">
-        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>111</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>108</v>
       </c>
       <c r="D4" t="s">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="E4">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5">
+        <v>5000</v>
+      </c>
+      <c r="F5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6">
+        <v>5000</v>
+      </c>
+      <c r="F6">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7">
+        <v>5000</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>108</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8">
+        <v>5000</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C9" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9">
+        <v>5000</v>
+      </c>
+      <c r="F9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10">
+        <v>5000</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C11" t="s">
+        <v>110</v>
+      </c>
+      <c r="D11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11">
+        <v>5000</v>
+      </c>
+      <c r="F11">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>114</v>
+      </c>
+      <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12">
+        <v>5000</v>
+      </c>
+      <c r="F12">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13">
+        <v>5000</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>79</v>
+      </c>
+      <c r="B14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14">
+        <v>5000</v>
+      </c>
+      <c r="F14">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C15" t="s">
+        <v>108</v>
+      </c>
+      <c r="D15" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15">
+        <v>5000</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E16">
+        <v>5000</v>
+      </c>
+      <c r="F16">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17">
+        <v>5000</v>
+      </c>
+      <c r="F17">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" t="s">
+        <v>126</v>
+      </c>
+      <c r="C18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18">
+        <v>5000</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>82</v>
+      </c>
+      <c r="B19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19">
+        <v>5000</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C20" t="s">
+        <v>110</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20">
+        <v>5000</v>
+      </c>
+      <c r="F20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" t="s">
+        <v>129</v>
+      </c>
+      <c r="C21" t="s">
+        <v>108</v>
+      </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C22" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" t="s">
+        <v>72</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
+      </c>
+      <c r="F22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>5000</v>
+      </c>
+      <c r="F23">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" t="s">
+        <v>108</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24">
+        <v>5000</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25">
+        <v>5000</v>
+      </c>
+      <c r="F25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26">
+        <v>5000</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B27" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" t="s">
+        <v>110</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27">
+        <v>5000</v>
+      </c>
+      <c r="F27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" t="s">
+        <v>136</v>
+      </c>
+      <c r="C28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28">
+        <v>5000</v>
+      </c>
+      <c r="F28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+      <c r="C29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D29" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29">
+        <v>5000</v>
+      </c>
+      <c r="F29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30">
+        <v>5000</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>69</v>
+      </c>
+      <c r="E31">
+        <v>5000</v>
+      </c>
+      <c r="F31">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32">
+        <v>5000</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+      <c r="C33" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33">
+        <v>5000</v>
+      </c>
+      <c r="F33">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+      <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" t="s">
+        <v>72</v>
+      </c>
+      <c r="E34">
+        <v>5000</v>
+      </c>
+      <c r="F34">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>89</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
+      </c>
+      <c r="C35" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" t="s">
+        <v>75</v>
+      </c>
+      <c r="E35">
+        <v>5000</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>144</v>
+      </c>
+      <c r="C36" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36">
+        <v>5000</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>145</v>
+      </c>
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>69</v>
+      </c>
+      <c r="E37">
+        <v>5000</v>
+      </c>
+      <c r="F37">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>91</v>
+      </c>
+      <c r="B38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38">
+        <v>5000</v>
+      </c>
+      <c r="F38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>72</v>
+      </c>
+      <c r="E39">
+        <v>5000</v>
+      </c>
+      <c r="F39">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>91</v>
+      </c>
+      <c r="B40" t="s">
+        <v>148</v>
+      </c>
+      <c r="C40" t="s">
+        <v>114</v>
+      </c>
+      <c r="D40" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40">
+        <v>5000</v>
+      </c>
+      <c r="F40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>92</v>
+      </c>
+      <c r="B41" t="s">
+        <v>149</v>
+      </c>
+      <c r="C41" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41">
+        <v>5000</v>
+      </c>
+      <c r="F41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" t="s">
+        <v>150</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" t="s">
+        <v>69</v>
+      </c>
+      <c r="E42">
+        <v>5000</v>
+      </c>
+      <c r="F42">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B43" t="s">
+        <v>151</v>
+      </c>
+      <c r="C43" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" t="s">
+        <v>72</v>
+      </c>
+      <c r="E43">
+        <v>5000</v>
+      </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" t="s">
+        <v>152</v>
+      </c>
+      <c r="C44" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44">
+        <v>5000</v>
+      </c>
+      <c r="F44">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" t="s">
+        <v>153</v>
+      </c>
+      <c r="C45" t="s">
+        <v>114</v>
+      </c>
+      <c r="D45" t="s">
+        <v>72</v>
+      </c>
+      <c r="E45">
+        <v>5000</v>
+      </c>
+      <c r="F45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E46">
+        <v>5000</v>
+      </c>
+      <c r="F46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>95</v>
+      </c>
+      <c r="B47" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47">
+        <v>5000</v>
+      </c>
+      <c r="F47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" t="s">
+        <v>110</v>
+      </c>
+      <c r="D48" t="s">
+        <v>69</v>
+      </c>
+      <c r="E48">
+        <v>5000</v>
+      </c>
+      <c r="F48">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" t="s">
+        <v>108</v>
+      </c>
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49">
+        <v>5000</v>
+      </c>
+      <c r="F49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
+        <v>158</v>
+      </c>
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50" t="s">
+        <v>72</v>
+      </c>
+      <c r="E50">
+        <v>5000</v>
+      </c>
+      <c r="F50">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C51" t="s">
+        <v>114</v>
+      </c>
+      <c r="D51" t="s">
+        <v>72</v>
+      </c>
+      <c r="E51">
+        <v>5000</v>
+      </c>
+      <c r="F51">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>97</v>
+      </c>
+      <c r="B52" t="s">
+        <v>160</v>
+      </c>
+      <c r="C52" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52">
+        <v>5000</v>
+      </c>
+      <c r="F52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s">
+        <v>110</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53">
+        <v>5000</v>
+      </c>
+      <c r="F53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" t="s">
+        <v>108</v>
+      </c>
+      <c r="D54" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54">
+        <v>5000</v>
+      </c>
+      <c r="F54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>98</v>
+      </c>
+      <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
+        <v>110</v>
+      </c>
+      <c r="D55" t="s">
+        <v>72</v>
+      </c>
+      <c r="E55">
+        <v>5000</v>
+      </c>
+      <c r="F55">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>98</v>
+      </c>
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
+        <v>114</v>
+      </c>
+      <c r="D56" t="s">
+        <v>72</v>
+      </c>
+      <c r="E56">
+        <v>5000</v>
+      </c>
+      <c r="F56">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B57" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" t="s">
+        <v>108</v>
+      </c>
+      <c r="D57" t="s">
+        <v>75</v>
+      </c>
+      <c r="E57">
+        <v>5000</v>
+      </c>
+      <c r="F57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>100</v>
+      </c>
+      <c r="B58" t="s">
+        <v>166</v>
+      </c>
+      <c r="C58" t="s">
+        <v>108</v>
+      </c>
+      <c r="D58" t="s">
+        <v>69</v>
+      </c>
+      <c r="E58">
+        <v>5000</v>
+      </c>
+      <c r="F58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>100</v>
+      </c>
+      <c r="B59" t="s">
+        <v>167</v>
+      </c>
+      <c r="C59" t="s">
+        <v>110</v>
+      </c>
+      <c r="D59" t="s">
+        <v>69</v>
+      </c>
+      <c r="E59">
+        <v>5000</v>
+      </c>
+      <c r="F59">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" t="s">
+        <v>168</v>
+      </c>
+      <c r="C60" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60">
+        <v>5000</v>
+      </c>
+      <c r="F60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" t="s">
+        <v>169</v>
+      </c>
+      <c r="C61" t="s">
+        <v>110</v>
+      </c>
+      <c r="D61" t="s">
+        <v>72</v>
+      </c>
+      <c r="E61">
+        <v>5000</v>
+      </c>
+      <c r="F61">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
+        <v>170</v>
+      </c>
+      <c r="C62" t="s">
+        <v>114</v>
+      </c>
+      <c r="D62" t="s">
+        <v>72</v>
+      </c>
+      <c r="E62">
+        <v>5000</v>
+      </c>
+      <c r="F62">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" t="s">
+        <v>171</v>
+      </c>
+      <c r="C63" t="s">
+        <v>108</v>
+      </c>
+      <c r="D63" t="s">
+        <v>75</v>
+      </c>
+      <c r="E63">
+        <v>5000</v>
+      </c>
+      <c r="F63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
+        <v>172</v>
+      </c>
+      <c r="C64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64" t="s">
+        <v>69</v>
+      </c>
+      <c r="E64">
+        <v>5000</v>
+      </c>
+      <c r="F64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>103</v>
+      </c>
+      <c r="B65" t="s">
+        <v>173</v>
+      </c>
+      <c r="C65" t="s">
+        <v>110</v>
+      </c>
+      <c r="D65" t="s">
+        <v>69</v>
+      </c>
+      <c r="E65">
+        <v>5000</v>
+      </c>
+      <c r="F65">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>104</v>
+      </c>
+      <c r="B66" t="s">
+        <v>174</v>
+      </c>
+      <c r="C66" t="s">
+        <v>108</v>
+      </c>
+      <c r="D66" t="s">
+        <v>72</v>
+      </c>
+      <c r="E66">
+        <v>5000</v>
+      </c>
+      <c r="F66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" t="s">
+        <v>175</v>
+      </c>
+      <c r="C67" t="s">
+        <v>110</v>
+      </c>
+      <c r="D67" t="s">
+        <v>72</v>
+      </c>
+      <c r="E67">
+        <v>5000</v>
+      </c>
+      <c r="F67">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" t="s">
+        <v>176</v>
+      </c>
+      <c r="C68" t="s">
+        <v>114</v>
+      </c>
+      <c r="D68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E68">
+        <v>5000</v>
+      </c>
+      <c r="F68">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>